<commit_message>
saved data to google bigquery table
</commit_message>
<xml_diff>
--- a/saved_data/data.xlsx
+++ b/saved_data/data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E88"/>
+  <dimension ref="A1:E92"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -463,22 +463,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Placebos</t>
+          <t>Fertility Technology</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Kathryn T Hall</t>
+          <t>Donna J. Drucker</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/placebos</t>
+          <t>https://mitpress.mit.edu/books/fertility-technology</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2022-09-20</t>
+          <t>2023-02-14</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -490,22 +490,22 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Happiness</t>
+          <t>Espionage</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Tim Lomas</t>
+          <t>Kristie Macrakis</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/happiness-1</t>
+          <t>https://mitpress.mit.edu/books/espionage</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2022-09-20</t>
+          <t>2023-02-14</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -517,22 +517,22 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Hunting</t>
+          <t>Causal Inference</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Jan Dizard, Mary Zeiss Stange</t>
+          <t>Paul R. Rosenbaum</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/hunting</t>
+          <t>https://mitpress.mit.edu/books/causal-inference</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2022-09-20</t>
+          <t>2023-02-14</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -544,22 +544,22 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Robot Ethics</t>
+          <t>Pragmatism</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Mark Coeckelbergh</t>
+          <t>John R. Shook</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/robot-ethics-1</t>
+          <t>https://mitpress.mit.edu/books/pragmatism</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2022-09-06</t>
+          <t>2023-02-07</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -571,22 +571,22 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Analog</t>
+          <t>Happiness</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Robert Hassan</t>
+          <t>Tim Lomas</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/analog</t>
+          <t>https://mitpress.mit.edu/books/happiness-1</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2022-09-06</t>
+          <t>2023-01-03</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -598,22 +598,22 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Whiteness</t>
+          <t>Analog</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Martin Lund</t>
+          <t>Robert Hassan</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/whiteness</t>
+          <t>https://mitpress.mit.edu/books/analog</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2022-09-06</t>
+          <t>2023-01-03</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -625,103 +625,103 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Neurolinguistics</t>
+          <t>Whiteness</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Giosuè Baggio</t>
+          <t>Martin Lund</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/neurolinguistics</t>
+          <t>https://mitpress.mit.edu/books/whiteness</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2022-05-10</t>
+          <t>2022-10-04</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>$15.95</t>
+          <t>$16.95</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Echo</t>
+          <t>Placebos</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Amit Pinchevski</t>
+          <t>Kathryn T Hall</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/echo</t>
+          <t>https://mitpress.mit.edu/books/placebos</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2022-05-10</t>
+          <t>2022-10-04</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>$15.95</t>
+          <t>$16.95</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Content</t>
+          <t>Hunting</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Kate Eichhorn</t>
+          <t>Jan Dizard, Mary Zeiss Stange</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/content</t>
+          <t>https://mitpress.mit.edu/books/hunting</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2022-05-10</t>
+          <t>2022-09-20</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>$15.95</t>
+          <t>$16.95</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Supernova</t>
+          <t>Robot Ethics</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Or Graur</t>
+          <t>Mark Coeckelbergh</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/supernova</t>
+          <t>https://mitpress.mit.edu/books/robot-ethics-1</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2022-02-08</t>
+          <t>2022-09-06</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -733,76 +733,76 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Nuclear Weapons</t>
+          <t>Neurolinguistics</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Mark Wolverton</t>
+          <t>Giosuè Baggio</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/nuclear-weapons</t>
+          <t>https://mitpress.mit.edu/books/neurolinguistics</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2022-02-01</t>
+          <t>2022-05-10</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>$16.95</t>
+          <t>$15.95</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Cybersecurity</t>
+          <t>Echo</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Duane C. Wilson</t>
+          <t>Amit Pinchevski</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/cybersecurity</t>
+          <t>https://mitpress.mit.edu/books/echo</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2021-09-14</t>
+          <t>2022-05-10</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>$15.95</t>
+          <t>$16.95</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Biofabrication</t>
+          <t>Content</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Ritu Raman</t>
+          <t>Kate Eichhorn</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/biofabrication</t>
+          <t>https://mitpress.mit.edu/books/content</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>2021-09-14</t>
+          <t>2022-05-10</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -814,76 +814,76 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>AI Assistants</t>
+          <t>Supernova</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Roberto Pieraccini</t>
+          <t>Or Graur</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/ai-assistants</t>
+          <t>https://mitpress.mit.edu/books/supernova</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>2021-09-07</t>
+          <t>2022-02-08</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>$15.95</t>
+          <t>$16.95</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Death and Dying</t>
+          <t>Nuclear Weapons</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Nicole Piemonte, Shawn Abreu</t>
+          <t>Mark Wolverton</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/death-and-dying</t>
+          <t>https://mitpress.mit.edu/books/nuclear-weapons</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>2021-09-07</t>
+          <t>2022-02-01</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>$15.95</t>
+          <t>$16.95</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Deconstruction</t>
+          <t>Biofabrication</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>David J. Gunkel</t>
+          <t>Ritu Raman</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/deconstruction</t>
+          <t>https://mitpress.mit.edu/books/biofabrication</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>2021-09-07</t>
+          <t>2021-09-14</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -895,22 +895,22 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Gender(s)</t>
+          <t>Cybersecurity</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Kathryn Bond Stockton</t>
+          <t>Duane C. Wilson</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/genders</t>
+          <t>https://mitpress.mit.edu/books/cybersecurity</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>2021-08-31</t>
+          <t>2021-09-14</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -922,22 +922,22 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>The Internet of Things, Revised And Updated Edition</t>
+          <t>Death and Dying</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Samuel Greengard</t>
+          <t>Nicole Piemonte, Shawn Abreu</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/internet-things-revised-and-updated-edition</t>
+          <t>https://mitpress.mit.edu/books/death-and-dying</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>2021-08-24</t>
+          <t>2021-09-07</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -949,22 +949,22 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Machine Learning, Revised And Updated Edition</t>
+          <t>AI Assistants</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Ethem Alpaydin</t>
+          <t>Roberto Pieraccini</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/machine-learning-revised-and-updated-edition</t>
+          <t>https://mitpress.mit.edu/books/ai-assistants</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>2021-08-17</t>
+          <t>2021-09-07</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -976,22 +976,22 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Annotation</t>
+          <t>Deconstruction</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Remi H. Kalir, Antero Garcia</t>
+          <t>David J. Gunkel</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/annotation</t>
+          <t>https://mitpress.mit.edu/books/deconstruction</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>2021-04-06</t>
+          <t>2021-09-07</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1003,22 +1003,22 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Hate Speech</t>
+          <t>Gender(s)</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Caitlin Ring Carlson</t>
+          <t>Kathryn Bond Stockton</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/hate-speech</t>
+          <t>https://mitpress.mit.edu/books/genders</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>2021-04-06</t>
+          <t>2021-08-31</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1030,22 +1030,22 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Science Fiction</t>
+          <t>The Internet of Things, Revised And Updated Edition</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Sherryl Vint</t>
+          <t>Samuel Greengard</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/science-fiction-2</t>
+          <t>https://mitpress.mit.edu/books/internet-things-revised-and-updated-edition</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>2021-02-16</t>
+          <t>2021-08-24</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -1057,22 +1057,22 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Ketamine</t>
+          <t>Machine Learning, Revised And Updated Edition</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Bita Moghaddam</t>
+          <t>Ethem Alpaydin</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/ketamine</t>
+          <t>https://mitpress.mit.edu/books/machine-learning-revised-and-updated-edition</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>2021-02-16</t>
+          <t>2021-08-17</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -1084,22 +1084,22 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Recommendation Engines</t>
+          <t>Hate Speech</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Michael Schrage</t>
+          <t>Caitlin Ring Carlson</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/recommendation-engines</t>
+          <t>https://mitpress.mit.edu/books/hate-speech</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>2020-09-01</t>
+          <t>2021-04-06</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -1111,22 +1111,22 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Behavioral Insights</t>
+          <t>Annotation</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Michael Hallsworth, Elspeth Kirkman</t>
+          <t>Remi H. Kalir, Antero Garcia</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/behavioral-insights</t>
+          <t>https://mitpress.mit.edu/books/annotation</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>2020-09-01</t>
+          <t>2021-04-06</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -1138,22 +1138,22 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Algorithms</t>
+          <t>Science Fiction</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Panos Louridas</t>
+          <t>Sherryl Vint</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/algorithms</t>
+          <t>https://mitpress.mit.edu/books/science-fiction-2</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>2020-08-18</t>
+          <t>2021-02-16</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -1165,22 +1165,22 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Visual Culture</t>
+          <t>Ketamine</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Alexis L. Boylan</t>
+          <t>Bita Moghaddam</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/visual-culture-1</t>
+          <t>https://mitpress.mit.edu/books/ketamine</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>2020-08-11</t>
+          <t>2021-02-16</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -1192,22 +1192,22 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Phenomenology</t>
+          <t>Recommendation Engines</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Chad Engelland</t>
+          <t>Michael Schrage</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/phenomenology</t>
+          <t>https://mitpress.mit.edu/books/recommendation-engines</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>2020-08-04</t>
+          <t>2020-09-01</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -1219,22 +1219,22 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Anticorruption</t>
+          <t>Behavioral Insights</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Robert I. Rotberg</t>
+          <t>Michael Hallsworth, Elspeth Kirkman</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/anticorruption</t>
+          <t>https://mitpress.mit.edu/books/behavioral-insights</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>2020-07-21</t>
+          <t>2020-09-01</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -1246,22 +1246,22 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Cynicism</t>
+          <t>Algorithms</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Ansgar Allen</t>
+          <t>Panos Louridas</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/cynicism</t>
+          <t>https://mitpress.mit.edu/books/algorithms</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>2020-04-14</t>
+          <t>2020-08-18</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -1273,22 +1273,22 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Contraception</t>
+          <t>Visual Culture</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Donna J. Drucker</t>
+          <t>Alexis L. Boylan</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/contraception</t>
+          <t>https://mitpress.mit.edu/books/visual-culture-1</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>2020-04-07</t>
+          <t>2020-08-11</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -1300,22 +1300,22 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>AI Ethics</t>
+          <t>Phenomenology</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Mark Coeckelbergh</t>
+          <t>Chad Engelland</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/ai-ethics</t>
+          <t>https://mitpress.mit.edu/books/phenomenology</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>2020-04-07</t>
+          <t>2020-08-04</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
@@ -1327,22 +1327,22 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Extraterrestrials</t>
+          <t>Anticorruption</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Wade Roush</t>
+          <t>Robert I. Rotberg</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/extraterrestrials</t>
+          <t>https://mitpress.mit.edu/books/anticorruption</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>2020-04-07</t>
+          <t>2020-07-21</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
@@ -1354,22 +1354,22 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Critical Thinking</t>
+          <t>Cynicism</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Jonathan Haber</t>
+          <t>Ansgar Allen</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/critical-thinking</t>
+          <t>https://mitpress.mit.edu/books/cynicism</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>2020-04-07</t>
+          <t>2020-04-14</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
@@ -1381,22 +1381,22 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Macroeconomics</t>
+          <t>Critical Thinking</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Felipe Larraín B.</t>
+          <t>Jonathan Haber</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/macroeconomics</t>
+          <t>https://mitpress.mit.edu/books/critical-thinking</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>2020-03-17</t>
+          <t>2020-04-07</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
@@ -1408,22 +1408,22 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>fMRI</t>
+          <t>Extraterrestrials</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Peter A. Bandettini</t>
+          <t>Wade Roush</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/fmri</t>
+          <t>https://mitpress.mit.edu/books/extraterrestrials</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>2020-02-25</t>
+          <t>2020-04-07</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
@@ -1435,22 +1435,22 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Quantum Entanglement</t>
+          <t>Contraception</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Jed Brody</t>
+          <t>Donna J. Drucker</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/quantum-entanglement</t>
+          <t>https://mitpress.mit.edu/books/contraception</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>2020-02-18</t>
+          <t>2020-04-07</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
@@ -1462,22 +1462,22 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Irony and Sarcasm</t>
+          <t>AI Ethics</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Roger Kreuz</t>
+          <t>Mark Coeckelbergh</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/irony-and-sarcasm</t>
+          <t>https://mitpress.mit.edu/books/ai-ethics</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>2020-02-18</t>
+          <t>2020-04-07</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
@@ -1489,22 +1489,22 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Collaborative Society</t>
+          <t>Macroeconomics</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Dariusz Jemielniak, Aleksandra Przegalinska</t>
+          <t>Felipe Larraín B.</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/collaborative-society</t>
+          <t>https://mitpress.mit.edu/books/macroeconomics</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>2020-02-18</t>
+          <t>2020-03-17</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
@@ -1516,22 +1516,22 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Spatial Computing</t>
+          <t>fMRI</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Shashi Shekhar, Pamela Vold</t>
+          <t>Peter A. Bandettini</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/spatial-computing</t>
+          <t>https://mitpress.mit.edu/books/fmri</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>2020-02-18</t>
+          <t>2020-02-25</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
@@ -1543,17 +1543,17 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Smart Cities</t>
+          <t>Collaborative Society</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Germaine Halegoua</t>
+          <t>Dariusz Jemielniak, Aleksandra Przegalinska</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/smart-cities</t>
+          <t>https://mitpress.mit.edu/books/collaborative-society</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -1570,22 +1570,22 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Recycling</t>
+          <t>Irony and Sarcasm</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Finn Arne Jørgensen</t>
+          <t>Roger Kreuz</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/recycling</t>
+          <t>https://mitpress.mit.edu/books/irony-and-sarcasm</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>2019-11-12</t>
+          <t>2020-02-18</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
@@ -1597,22 +1597,22 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Citizenship</t>
+          <t>Quantum Entanglement</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Dimitry Kochenov</t>
+          <t>Jed Brody</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/citizenship</t>
+          <t>https://mitpress.mit.edu/books/quantum-entanglement</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>2019-11-12</t>
+          <t>2020-02-18</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
@@ -1624,22 +1624,22 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Deep Learning</t>
+          <t>Spatial Computing</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>John D. Kelleher</t>
+          <t>Shashi Shekhar, Pamela Vold</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/deep-learning-1</t>
+          <t>https://mitpress.mit.edu/books/spatial-computing</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>2019-09-10</t>
+          <t>2020-02-18</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
@@ -1651,22 +1651,22 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Fake Photos</t>
+          <t>Smart Cities</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>Hany Farid</t>
+          <t>Germaine Halegoua</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/fake-photos</t>
+          <t>https://mitpress.mit.edu/books/smart-cities</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>2019-09-10</t>
+          <t>2020-02-18</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
@@ -1678,22 +1678,22 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Nihilism</t>
+          <t>Recycling</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Nolen Gertz</t>
+          <t>Finn Arne Jørgensen</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/nihilism</t>
+          <t>https://mitpress.mit.edu/books/recycling</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>2019-09-10</t>
+          <t>2019-11-12</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
@@ -1705,22 +1705,22 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Virtual Reality</t>
+          <t>Citizenship</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Samuel Greengard</t>
+          <t>Dimitry Kochenov</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/virtual-reality</t>
+          <t>https://mitpress.mit.edu/books/citizenship</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>2019-09-10</t>
+          <t>2019-11-12</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
@@ -1732,22 +1732,22 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Food</t>
+          <t>Fake Photos</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Fabio Parasecoli</t>
+          <t>Hany Farid</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/food-1</t>
+          <t>https://mitpress.mit.edu/books/fake-photos</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>2019-05-21</t>
+          <t>2019-09-10</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
@@ -1759,22 +1759,22 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Computational Thinking</t>
+          <t>Nihilism</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Peter J. Denning, Matti Tedre</t>
+          <t>Nolen Gertz</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/computational-thinking</t>
+          <t>https://mitpress.mit.edu/books/nihilism</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>2019-05-14</t>
+          <t>2019-09-10</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
@@ -1786,22 +1786,22 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Sexual Consent</t>
+          <t>Virtual Reality</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Milena Popova</t>
+          <t>Samuel Greengard</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/sexual-consent</t>
+          <t>https://mitpress.mit.edu/books/virtual-reality</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>2019-05-07</t>
+          <t>2019-09-10</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
@@ -1813,22 +1813,22 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>3D Printing</t>
+          <t>Deep Learning</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>John M. Jordan</t>
+          <t>John D. Kelleher</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/3d-printing</t>
+          <t>https://mitpress.mit.edu/books/deep-learning-1</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>2019-03-12</t>
+          <t>2019-09-10</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
@@ -1840,22 +1840,22 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>GPS</t>
+          <t>Food</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Paul E. Ceruzzi</t>
+          <t>Fabio Parasecoli</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/gps</t>
+          <t>https://mitpress.mit.edu/books/food-1</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>2018-11-06</t>
+          <t>2019-05-21</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
@@ -1867,22 +1867,22 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Spaceflight</t>
+          <t>Computational Thinking</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Michael J. Neufeld</t>
+          <t>Peter J. Denning, Matti Tedre</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/spaceflight</t>
+          <t>https://mitpress.mit.edu/books/computational-thinking</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>2018-10-16</t>
+          <t>2019-05-14</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
@@ -1894,22 +1894,22 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>School Choice</t>
+          <t>Sexual Consent</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>David R. Garcia</t>
+          <t>Milena Popova</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/school-choice</t>
+          <t>https://mitpress.mit.edu/books/sexual-consent</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>2018-09-18</t>
+          <t>2019-05-07</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
@@ -1921,22 +1921,22 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Carbon Capture</t>
+          <t>3D Printing</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Howard J. Herzog</t>
+          <t>John M. Jordan</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/carbon-capture</t>
+          <t>https://mitpress.mit.edu/books/3d-printing</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>2018-09-11</t>
+          <t>2019-03-12</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
@@ -1948,22 +1948,22 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Haptics</t>
+          <t>GPS</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Lynette Jones</t>
+          <t>Paul E. Ceruzzi</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/haptics</t>
+          <t>https://mitpress.mit.edu/books/gps</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>2018-09-04</t>
+          <t>2018-11-06</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
@@ -1975,49 +1975,49 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Extremism</t>
+          <t>Spaceflight</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>J. M. Berger</t>
+          <t>Michael J. Neufeld</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/extremism</t>
+          <t>https://mitpress.mit.edu/books/spaceflight</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>2018-08-28</t>
+          <t>2018-10-16</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>$16.95</t>
+          <t>$15.95</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>The Book</t>
+          <t>School Choice</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Amaranth Borsuk</t>
+          <t>David R. Garcia</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/book</t>
+          <t>https://mitpress.mit.edu/books/school-choice</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>2018-05-04</t>
+          <t>2018-09-18</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
@@ -2029,49 +2029,49 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Data Science</t>
+          <t>Carbon Capture</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>John D. Kelleher, Brendan Tierney</t>
+          <t>Howard J. Herzog</t>
         </is>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/data-science</t>
+          <t>https://mitpress.mit.edu/books/carbon-capture</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>2018-04-13</t>
+          <t>2018-09-11</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>$15.95</t>
+          <t>$16.95</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Synesthesia</t>
+          <t>Haptics</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Richard E. Cytowic</t>
+          <t>Lynette Jones</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/synesthesia</t>
+          <t>https://mitpress.mit.edu/books/haptics</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>2018-03-09</t>
+          <t>2018-09-04</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
@@ -2083,76 +2083,76 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Post-Truth</t>
+          <t>Extremism</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>Lee McIntyre</t>
+          <t>J. M. Berger</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/post-truth</t>
+          <t>https://mitpress.mit.edu/books/extremism</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>2018-02-16</t>
+          <t>2018-08-28</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>$15.95</t>
+          <t>$16.95</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>The Future</t>
+          <t>The Book</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Nick Montfort</t>
+          <t>Amaranth Borsuk</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/future</t>
+          <t>https://mitpress.mit.edu/books/book</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>2017-12-08</t>
+          <t>2018-05-04</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>$15.95</t>
+          <t>$16.95</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Machine Translation</t>
+          <t>Data Science</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>Thierry Poibeau</t>
+          <t>John D. Kelleher, Brendan Tierney</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/machine-translation-1</t>
+          <t>https://mitpress.mit.edu/books/data-science</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>2017-09-15</t>
+          <t>2018-04-13</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
@@ -2164,22 +2164,22 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Information and Society</t>
+          <t>Synesthesia</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Michael Buckland</t>
+          <t>Richard E. Cytowic</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/information-and-society</t>
+          <t>https://mitpress.mit.edu/books/synesthesia</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>2017-03-03</t>
+          <t>2018-03-09</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
@@ -2191,22 +2191,22 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Robots</t>
+          <t>Post-Truth</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>John M. Jordan</t>
+          <t>Lee McIntyre</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/robots</t>
+          <t>https://mitpress.mit.edu/books/post-truth</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>2016-10-14</t>
+          <t>2018-02-16</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
@@ -2218,22 +2218,22 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Machine Learning</t>
+          <t>The Future</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Ethem Alpaydin</t>
+          <t>Nick Montfort</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/machine-learning</t>
+          <t>https://mitpress.mit.edu/books/future</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>2016-10-07</t>
+          <t>2017-12-08</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
@@ -2245,76 +2245,76 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>The Mind–Body Problem</t>
+          <t>Machine Translation</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Jonathan Westphal</t>
+          <t>Thierry Poibeau</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/mind-body-problem</t>
+          <t>https://mitpress.mit.edu/books/machine-translation-1</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>2016-09-30</t>
+          <t>2017-09-15</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>$16.95</t>
+          <t>$15.95</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Neuroplasticity</t>
+          <t>Information and Society</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Moheb Costandi</t>
+          <t>Michael Buckland</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/neuroplasticity</t>
+          <t>https://mitpress.mit.edu/books/information-and-society</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>2016-08-19</t>
+          <t>2017-03-03</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>$16.95</t>
+          <t>$15.95</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Self-Tracking</t>
+          <t>Robots</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>Gina Neff, Dawn Nafus</t>
+          <t>John M. Jordan</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/self-tracking</t>
+          <t>https://mitpress.mit.edu/books/robots</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>2016-06-24</t>
+          <t>2016-10-14</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
@@ -2326,22 +2326,22 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Cloud Computing</t>
+          <t>Machine Learning</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>Nayan B. Ruparelia</t>
+          <t>Ethem Alpaydin</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/cloud-computing</t>
+          <t>https://mitpress.mit.edu/books/machine-learning</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>2016-05-13</t>
+          <t>2016-10-07</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
@@ -2353,76 +2353,76 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Auctions</t>
+          <t>The Mind–Body Problem</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Timothy P. Hubbard, Harry J. Paarsch</t>
+          <t>Jonathan Westphal</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/auctions</t>
+          <t>https://mitpress.mit.edu/books/mind-body-problem</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>2016-01-06</t>
+          <t>2016-09-30</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>$15.95</t>
+          <t>$16.95</t>
         </is>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Metadata</t>
+          <t>Neuroplasticity</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Jeffrey Pomerantz</t>
+          <t>Moheb Costandi</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/metadata</t>
+          <t>https://mitpress.mit.edu/books/neuroplasticity</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>2015-11-06</t>
+          <t>2016-08-19</t>
         </is>
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>$15.95</t>
+          <t>$16.95</t>
         </is>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Sustainability</t>
+          <t>Self-Tracking</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>Kent E. Portney</t>
+          <t>Gina Neff, Dawn Nafus</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/sustainability</t>
+          <t>https://mitpress.mit.edu/books/self-tracking</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>2015-10-09</t>
+          <t>2016-06-24</t>
         </is>
       </c>
       <c r="E74" t="inlineStr">
@@ -2434,49 +2434,49 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>The Technological Singularity</t>
+          <t>Cloud Computing</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>Murray Shanahan</t>
+          <t>Nayan B. Ruparelia</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/technological-singularity</t>
+          <t>https://mitpress.mit.edu/books/cloud-computing</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>2015-08-07</t>
+          <t>2016-05-13</t>
         </is>
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>$16.95</t>
+          <t>$15.95</t>
         </is>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>The Internet of Things</t>
+          <t>Auctions</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Samuel Greengard</t>
+          <t>Timothy P. Hubbard, Harry J. Paarsch</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/internet-things</t>
+          <t>https://mitpress.mit.edu/books/auctions</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>2015-03-20</t>
+          <t>2016-01-06</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
@@ -2488,76 +2488,76 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>MOOCs</t>
+          <t>Metadata</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>Jonathan Haber</t>
+          <t>Jeffrey Pomerantz</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/moocs</t>
+          <t>https://mitpress.mit.edu/books/metadata</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>2014-09-26</t>
+          <t>2015-11-06</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>$15.95</t>
+          <t>$16.95</t>
         </is>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Understanding Beliefs</t>
+          <t>Sustainability</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Nils J. Nilsson</t>
+          <t>Kent E. Portney</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/understanding-beliefs</t>
+          <t>https://mitpress.mit.edu/books/sustainability</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
         <is>
-          <t>2014-08-15</t>
+          <t>2015-10-09</t>
         </is>
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>$16.95</t>
+          <t>$15.95</t>
         </is>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>The Conscious Mind</t>
+          <t>The Technological Singularity</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Zoltan Torey</t>
+          <t>Murray Shanahan</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/conscious-mind</t>
+          <t>https://mitpress.mit.edu/books/technological-singularity</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>2014-08-08</t>
+          <t>2015-08-07</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
@@ -2569,22 +2569,22 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Paradox</t>
+          <t>The Internet of Things</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>Margaret Cuonzo</t>
+          <t>Samuel Greengard</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/paradox</t>
+          <t>https://mitpress.mit.edu/books/internet-things</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>2014-02-14</t>
+          <t>2015-03-20</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
@@ -2596,22 +2596,22 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Free Will</t>
+          <t>MOOCs</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Mark Balaguer</t>
+          <t>Jonathan Haber</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/free-will</t>
+          <t>https://mitpress.mit.edu/books/moocs</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
         <is>
-          <t>2014-02-14</t>
+          <t>2014-09-26</t>
         </is>
       </c>
       <c r="E81" t="inlineStr">
@@ -2623,103 +2623,103 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Memes in Digital Culture</t>
+          <t>Understanding Beliefs</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Limor Shifman</t>
+          <t>Nils J. Nilsson</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/memes-digital-culture</t>
+          <t>https://mitpress.mit.edu/books/understanding-beliefs</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
         <is>
-          <t>2013-10-04</t>
+          <t>2014-08-15</t>
         </is>
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>$15.95</t>
+          <t>$16.95</t>
         </is>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Crowdsourcing</t>
+          <t>The Conscious Mind</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Daren C. Brabham</t>
+          <t>Zoltan Torey</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/crowdsourcing</t>
+          <t>https://mitpress.mit.edu/books/conscious-mind</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>2013-05-10</t>
+          <t>2014-08-08</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>$15.95</t>
+          <t>$16.95</t>
         </is>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Waves</t>
+          <t>Paradox</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Fredric Raichlen</t>
+          <t>Margaret Cuonzo</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/waves</t>
+          <t>https://mitpress.mit.edu/books/paradox</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>2012-10-19</t>
+          <t>2014-02-14</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>$16.95</t>
+          <t>$15.95</t>
         </is>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Open Access</t>
+          <t>Free Will</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Peter Suber</t>
+          <t>Mark Balaguer</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/open-access</t>
+          <t>https://mitpress.mit.edu/books/free-will</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
         <is>
-          <t>2012-07-20</t>
+          <t>2014-02-14</t>
         </is>
       </c>
       <c r="E85" t="inlineStr">
@@ -2731,49 +2731,49 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Computing</t>
+          <t>Memes in Digital Culture</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Paul E. Ceruzzi</t>
+          <t>Limor Shifman</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/computing-1</t>
+          <t>https://mitpress.mit.edu/books/memes-digital-culture</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
         <is>
-          <t>2012-06-15</t>
+          <t>2013-10-04</t>
         </is>
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>$16.95</t>
+          <t>$15.95</t>
         </is>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Information and the Modern Corporation</t>
+          <t>Crowdsourcing</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>James W. Cortada</t>
+          <t>Daren C. Brabham</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/information-and-modern-corporation</t>
+          <t>https://mitpress.mit.edu/books/crowdsourcing</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
         <is>
-          <t>2011-10-07</t>
+          <t>2013-05-10</t>
         </is>
       </c>
       <c r="E87" t="inlineStr">
@@ -2785,25 +2785,133 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
+          <t>Waves</t>
+        </is>
+      </c>
+      <c r="B88" t="inlineStr">
+        <is>
+          <t>Fredric Raichlen</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>https://mitpress.mit.edu/books/waves</t>
+        </is>
+      </c>
+      <c r="D88" t="inlineStr">
+        <is>
+          <t>2012-10-19</t>
+        </is>
+      </c>
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>$16.95</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>Open Access</t>
+        </is>
+      </c>
+      <c r="B89" t="inlineStr">
+        <is>
+          <t>Peter Suber</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>https://mitpress.mit.edu/books/open-access</t>
+        </is>
+      </c>
+      <c r="D89" t="inlineStr">
+        <is>
+          <t>2012-07-20</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>$15.95</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>Computing</t>
+        </is>
+      </c>
+      <c r="B90" t="inlineStr">
+        <is>
+          <t>Paul E. Ceruzzi</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>https://mitpress.mit.edu/books/computing-1</t>
+        </is>
+      </c>
+      <c r="D90" t="inlineStr">
+        <is>
+          <t>2012-06-15</t>
+        </is>
+      </c>
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>$16.95</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>Information and the Modern Corporation</t>
+        </is>
+      </c>
+      <c r="B91" t="inlineStr">
+        <is>
+          <t>James W. Cortada</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>https://mitpress.mit.edu/books/information-and-modern-corporation</t>
+        </is>
+      </c>
+      <c r="D91" t="inlineStr">
+        <is>
+          <t>2011-10-07</t>
+        </is>
+      </c>
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>$15.95</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
           <t>Intellectual Property Strategy</t>
         </is>
       </c>
-      <c r="B88" t="inlineStr">
+      <c r="B92" t="inlineStr">
         <is>
           <t>John Palfrey</t>
         </is>
       </c>
-      <c r="C88" t="inlineStr">
+      <c r="C92" t="inlineStr">
         <is>
           <t>https://mitpress.mit.edu/books/intellectual-property-strategy</t>
         </is>
       </c>
-      <c r="D88" t="inlineStr">
+      <c r="D92" t="inlineStr">
         <is>
           <t>2011-10-07</t>
         </is>
       </c>
-      <c r="E88" t="inlineStr">
+      <c r="E92" t="inlineStr">
         <is>
           <t>$15.95</t>
         </is>

</xml_diff>

<commit_message>
rewrote script because the url changed
</commit_message>
<xml_diff>
--- a/saved_data/data.xlsx
+++ b/saved_data/data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E92"/>
+  <dimension ref="A1:H70"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,1183 +441,1757 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>link</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
           <t>authors</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>link</t>
-        </is>
-      </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>authors_webpage</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>publish_date</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>book_length</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>price</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>purchase_links</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Fertility Technology</t>
+          <t>The Future</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Donna J. Drucker</t>
+          <t>https://mitpress.mit.edu/9780262534819/the-future</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/fertility-technology</t>
+          <t>Nick Montfort</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2023-02-14</t>
+          <t>https://mitpress.mit.edu/author/nick-montfort-4107</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>$16.95</t>
+          <t>December 8, 2017</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>192</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>$15.95</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>https://www.penguinrandomhouse.com/search/site/?q=9780262534819</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Espionage</t>
+          <t>Critical Thinking</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Kristie Macrakis</t>
+          <t>https://mitpress.mit.edu/9780262538282/critical-thinking</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/espionage</t>
+          <t>Jonathan Haber</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2023-02-14</t>
+          <t>https://mitpress.mit.edu/author/jonathan-haber-21957</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>$16.95</t>
+          <t>April 7, 2020</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>232</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>$15.95</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>https://www.penguinrandomhouse.com/search/site/?q=9780262538282</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Causal Inference</t>
+          <t>Hunting</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Paul R. Rosenbaum</t>
+          <t>https://mitpress.mit.edu/9780262543293/hunting</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/causal-inference</t>
+          <t>Jan E. Dizard &amp; Mary Zeiss Stange</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>2023-02-14</t>
+          <t>https://mitpress.mit.edu/author/jan-e-dizard-34146 &amp; https://mitpress.mit.edu/author/mary-zeiss-stange-34147</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
+          <t>October 4, 2022</t>
+        </is>
+      </c>
+      <c r="F4" t="n">
+        <v>248</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
           <t>$16.95</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>https://www.penguinrandomhouse.com/search/site/?q=9780262543293</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Pragmatism</t>
+          <t>Content</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>John R. Shook</t>
+          <t>https://mitpress.mit.edu/9780262543286/content</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/pragmatism</t>
+          <t>Kate Eichhorn</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2023-02-07</t>
+          <t>https://mitpress.mit.edu/author/kate-eichhorn-21842</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>$16.95</t>
+          <t>May 10, 2022</t>
+        </is>
+      </c>
+      <c r="F5" t="n">
+        <v>192</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>$15.95</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>https://www.penguinrandomhouse.com/search/site/?q=9780262543286</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Happiness</t>
+          <t>Machine Learning, revised and updated edition</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Tim Lomas</t>
+          <t>https://mitpress.mit.edu/9780262542524/machine-learning</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/happiness-1</t>
+          <t>Ethem Alpaydın</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>2023-01-03</t>
+          <t>https://mitpress.mit.edu/author/ethem-alpaydn-1089</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>$16.95</t>
+          <t>August 17, 2021</t>
+        </is>
+      </c>
+      <c r="F6" t="n">
+        <v>280</v>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>$15.95</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>https://www.penguinrandomhouse.com/search/site/?q=9780262542524</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Analog</t>
+          <t>Macroeconomics</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Robert Hassan</t>
+          <t>https://mitpress.mit.edu/9780262538572/macroeconomics</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/analog</t>
+          <t>Felipe Larraín B.</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>2023-01-03</t>
+          <t>https://mitpress.mit.edu/author/felipe-larrain-b-13187</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>$16.95</t>
+          <t>March 17, 2020</t>
+        </is>
+      </c>
+      <c r="F7" t="n">
+        <v>296</v>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>$15.95</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>https://www.penguinrandomhouse.com/search/site/?q=9780262538572</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Whiteness</t>
+          <t>fMRI</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Martin Lund</t>
+          <t>https://mitpress.mit.edu/9780262538039/fmri</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/whiteness</t>
+          <t>Peter A. Bandettini</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>2022-10-04</t>
+          <t>https://mitpress.mit.edu/author/peter-a-bandettini-15778</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>$16.95</t>
+          <t>February 25, 2020</t>
+        </is>
+      </c>
+      <c r="F8" t="n">
+        <v>280</v>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>$15.95</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>https://www.penguinrandomhouse.com/search/site/?q=9780262538039</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Placebos</t>
+          <t>Collaborative Society</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Kathryn T Hall</t>
+          <t>https://mitpress.mit.edu/9780262537919/collaborative-society</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/placebos</t>
+          <t>Dariusz Jemielniak &amp; Aleksandra Przegalinska</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>2022-10-04</t>
+          <t>https://mitpress.mit.edu/author/dariusz-jemielniak-19785 &amp; https://mitpress.mit.edu/author/aleksandra-przegalinska-28238</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>$16.95</t>
+          <t>February 18, 2020</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
+        <v>256</v>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>$15.95</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>https://www.penguinrandomhouse.com/search/site/?q=9780262537919</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Hunting</t>
+          <t>GPS</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Jan Dizard, Mary Zeiss Stange</t>
+          <t>https://mitpress.mit.edu/9780262535953/gps</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/hunting</t>
+          <t>Paul E. Ceruzzi</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>2022-09-20</t>
+          <t>https://mitpress.mit.edu/author/paul-e-ceruzzi-4023</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>$16.95</t>
+          <t>November 6, 2018</t>
+        </is>
+      </c>
+      <c r="F10" t="n">
+        <v>232</v>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>$15.95</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>https://www.penguinrandomhouse.com/search/site/?q=9780262535953</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Robot Ethics</t>
+          <t>School Choice</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Mark Coeckelbergh</t>
+          <t>https://mitpress.mit.edu/9780262535908/school-choice</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/robot-ethics-1</t>
+          <t>David R. Garcia</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>2022-09-06</t>
+          <t>https://mitpress.mit.edu/author/david-r-garcia-28397</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>$16.95</t>
+          <t>September 18, 2018</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
+        <v>216</v>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>$15.95</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>https://www.penguinrandomhouse.com/search/site/?q=9780262535908</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Neurolinguistics</t>
+          <t>Haptics</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Giosuè Baggio</t>
+          <t>https://mitpress.mit.edu/9780262535809/haptics</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/neurolinguistics</t>
+          <t>Lynette Jones</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>2022-05-10</t>
+          <t>https://mitpress.mit.edu/author/lynette-jones-26298</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>$15.95</t>
+          <t>September 4, 2018</t>
+        </is>
+      </c>
+      <c r="F12" t="n">
+        <v>192</v>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>$15.95</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>https://www.penguinrandomhouse.com/search/site/?q=9780262535809</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Echo</t>
+          <t>Machine Translation</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Amit Pinchevski</t>
+          <t>https://mitpress.mit.edu/9780262534215/machine-translation</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/echo</t>
+          <t>Thierry Poibeau</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>2022-05-10</t>
+          <t>https://mitpress.mit.edu/author/thierry-poibeau-24043</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>$16.95</t>
+          <t>September 15, 2017</t>
+        </is>
+      </c>
+      <c r="F13" t="n">
+        <v>296</v>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>$15.95</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>https://www.penguinrandomhouse.com/search/site/?q=9780262534215</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Content</t>
+          <t>Paradox</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Kate Eichhorn</t>
+          <t>https://mitpress.mit.edu/9780262525497/paradox</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/content</t>
+          <t>Margaret Cuonzo</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>2022-05-10</t>
+          <t>https://mitpress.mit.edu/author/margaret-cuonzo-20791</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>$15.95</t>
+          <t>February 14, 2014</t>
+        </is>
+      </c>
+      <c r="F14" t="n">
+        <v>240</v>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>$15.95</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>https://www.penguinrandomhouse.com/search/site/?q=9780262525497</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Supernova</t>
+          <t>Analog</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Or Graur</t>
+          <t>https://mitpress.mit.edu/9780262544498/analog</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/supernova</t>
+          <t>Robert Hassan</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>2022-02-08</t>
+          <t>https://mitpress.mit.edu/author/robert-hassan-22991</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
+          <t>January 3, 2023</t>
+        </is>
+      </c>
+      <c r="F15" t="n">
+        <v>272</v>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
           <t>$16.95</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>https://www.penguinrandomhouse.com/search/site/?q=9780262544498</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Nuclear Weapons</t>
+          <t>Happiness</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Mark Wolverton</t>
+          <t>https://mitpress.mit.edu/9780262544207/happiness</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/nuclear-weapons</t>
+          <t>Tim Lomas</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>2022-02-01</t>
+          <t>https://mitpress.mit.edu/author/tim-lomas-26931</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
+          <t>January 3, 2023</t>
+        </is>
+      </c>
+      <c r="F16" t="n">
+        <v>304</v>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
           <t>$16.95</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>https://www.penguinrandomhouse.com/search/site/?q=9780262544207</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Biofabrication</t>
+          <t>Placebos</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Ritu Raman</t>
+          <t>https://mitpress.mit.edu/9780262544252/placebos</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/biofabrication</t>
+          <t>Kathryn T Hall</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>2021-09-14</t>
+          <t>https://mitpress.mit.edu/author/kathryn-t-hall-33978</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>$15.95</t>
+          <t>October 4, 2022</t>
+        </is>
+      </c>
+      <c r="F17" t="n">
+        <v>216</v>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>$16.95</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>https://www.penguinrandomhouse.com/search/site/?q=9780262544252</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Cybersecurity</t>
+          <t>Whiteness</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Duane C. Wilson</t>
+          <t>https://mitpress.mit.edu/9780262544191/whiteness</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/cybersecurity</t>
+          <t>Martin Lund</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>2021-09-14</t>
+          <t>https://mitpress.mit.edu/author/martin-lund-34553</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>$15.95</t>
+          <t>October 4, 2022</t>
+        </is>
+      </c>
+      <c r="F18" t="n">
+        <v>272</v>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>$16.95</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>https://www.penguinrandomhouse.com/search/site/?q=9780262544191</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Death and Dying</t>
+          <t>Robot Ethics</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Nicole Piemonte, Shawn Abreu</t>
+          <t>https://mitpress.mit.edu/9780262544092/robot-ethics</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/death-and-dying</t>
+          <t>Mark Coeckelbergh</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>2021-09-07</t>
+          <t>https://mitpress.mit.edu/author/mark-coeckelbergh-25812</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>$15.95</t>
+          <t>September 6, 2022</t>
+        </is>
+      </c>
+      <c r="F19" t="n">
+        <v>272</v>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>$16.95</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>https://www.penguinrandomhouse.com/search/site/?q=9780262544092</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>AI Assistants</t>
+          <t>Neurolinguistics</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Roberto Pieraccini</t>
+          <t>https://mitpress.mit.edu/9780262543262/neurolinguistics</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/ai-assistants</t>
+          <t>Giosuè Baggio</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>2021-09-07</t>
+          <t>https://mitpress.mit.edu/author/giosue-baggio-12851</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>$15.95</t>
+          <t>May 10, 2022</t>
+        </is>
+      </c>
+      <c r="F20" t="n">
+        <v>224</v>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>$15.95</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>https://www.penguinrandomhouse.com/search/site/?q=9780262543262</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Deconstruction</t>
+          <t>Echo</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>David J. Gunkel</t>
+          <t>https://mitpress.mit.edu/9780262543408/echo</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/deconstruction</t>
+          <t>Amit Pinchevski</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>2021-09-07</t>
+          <t>https://mitpress.mit.edu/author/amit-pinchevski-33388</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>$15.95</t>
+          <t>May 10, 2022</t>
+        </is>
+      </c>
+      <c r="F21" t="n">
+        <v>232</v>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>$16.95</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>https://www.penguinrandomhouse.com/search/site/?q=9780262543408</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Gender(s)</t>
+          <t>Supernova</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Kathryn Bond Stockton</t>
+          <t>https://mitpress.mit.edu/9780262543149/supernova</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/genders</t>
+          <t>Or Graur</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>2021-08-31</t>
+          <t>https://mitpress.mit.edu/author/or-graur-32668</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>$15.95</t>
+          <t>February 8, 2022</t>
+        </is>
+      </c>
+      <c r="F22" t="n">
+        <v>240</v>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>$16.95</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>https://www.penguinrandomhouse.com/search/site/?q=9780262543149</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>The Internet of Things, Revised And Updated Edition</t>
+          <t>Nuclear Weapons</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Samuel Greengard</t>
+          <t>https://mitpress.mit.edu/9780262543316/nuclear-weapons</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/internet-things-revised-and-updated-edition</t>
+          <t>Mark Wolverton</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>2021-08-24</t>
+          <t>https://mitpress.mit.edu/author/mark-wolverton-28331</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>$15.95</t>
+          <t>February 1, 2022</t>
+        </is>
+      </c>
+      <c r="F23" t="n">
+        <v>280</v>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>$16.95</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>https://www.penguinrandomhouse.com/search/site/?q=9780262543316</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Machine Learning, Revised And Updated Edition</t>
+          <t>Cybersecurity</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>Ethem Alpaydin</t>
+          <t>https://mitpress.mit.edu/9780262542548/cybersecurity</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/machine-learning-revised-and-updated-edition</t>
+          <t>Duane C. Wilson</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>2021-08-17</t>
+          <t>https://mitpress.mit.edu/author/duane-c-wilson-28430</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>$15.95</t>
+          <t>September 14, 2021</t>
+        </is>
+      </c>
+      <c r="F24" t="n">
+        <v>160</v>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>$15.95</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>https://www.penguinrandomhouse.com/search/site/?q=9780262542548</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Hate Speech</t>
+          <t>Biofabrication</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>Caitlin Ring Carlson</t>
+          <t>https://mitpress.mit.edu/9780262542968/biofabrication</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/hate-speech</t>
+          <t>Ritu Raman</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>2021-04-06</t>
+          <t>https://mitpress.mit.edu/author/ritu-raman-32773</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>$15.95</t>
+          <t>September 14, 2021</t>
+        </is>
+      </c>
+      <c r="F25" t="n">
+        <v>216</v>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>$15.95</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>https://www.penguinrandomhouse.com/search/site/?q=9780262542968</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Annotation</t>
+          <t>Death and Dying</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>Remi H. Kalir, Antero Garcia</t>
+          <t>https://mitpress.mit.edu/9780262542425/death-and-dying</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/annotation</t>
+          <t>Nicole Piemonte &amp; Shawn Abreu</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>2021-04-06</t>
+          <t>https://mitpress.mit.edu/author/nicole-piemonte-27774 &amp; https://mitpress.mit.edu/author/shawn-abreu-31775</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>$15.95</t>
+          <t>September 7, 2021</t>
+        </is>
+      </c>
+      <c r="F26" t="n">
+        <v>248</v>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>$15.95</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>https://www.penguinrandomhouse.com/search/site/?q=9780262542425</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Science Fiction</t>
+          <t>AI Assistants</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>Sherryl Vint</t>
+          <t>https://mitpress.mit.edu/9780262542555/ai-assistants</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/science-fiction-2</t>
+          <t>Roberto Pieraccini</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>2021-02-16</t>
+          <t>https://mitpress.mit.edu/author/roberto-pieraccini-16458</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>$15.95</t>
+          <t>September 7, 2021</t>
+        </is>
+      </c>
+      <c r="F27" t="n">
+        <v>288</v>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>$15.95</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>https://www.penguinrandomhouse.com/search/site/?q=9780262542555</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Ketamine</t>
+          <t>Deconstruction</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>Bita Moghaddam</t>
+          <t>https://mitpress.mit.edu/9780262542470/deconstruction</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/ketamine</t>
+          <t>David J. Gunkel</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>2021-02-16</t>
+          <t>https://mitpress.mit.edu/author/david-j-gunkel-16058</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>$15.95</t>
+          <t>September 7, 2021</t>
+        </is>
+      </c>
+      <c r="F28" t="n">
+        <v>200</v>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>$15.95</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>https://www.penguinrandomhouse.com/search/site/?q=9780262542470</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Recommendation Engines</t>
+          <t>Gender(s)</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Michael Schrage</t>
+          <t>https://mitpress.mit.edu/9780262542609/genders</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/recommendation-engines</t>
+          <t>Kathryn Bond Stockton</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>2020-09-01</t>
+          <t>https://mitpress.mit.edu/author/kathryn-bond-stockton-34573</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>$15.95</t>
+          <t>August 31, 2021</t>
+        </is>
+      </c>
+      <c r="F29" t="n">
+        <v>256</v>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>$15.95</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>https://www.penguinrandomhouse.com/search/site/?q=9780262542609</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Behavioral Insights</t>
+          <t>The Internet of Things, revised and updated edition</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Michael Hallsworth, Elspeth Kirkman</t>
+          <t>https://mitpress.mit.edu/9780262542623/the-internet-of-things</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/behavioral-insights</t>
+          <t>Samuel Greengard</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>2020-09-01</t>
+          <t>https://mitpress.mit.edu/author/samuel-greengard-22712</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>$15.95</t>
+          <t>August 24, 2021</t>
+        </is>
+      </c>
+      <c r="F30" t="n">
+        <v>296</v>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>$15.95</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>https://www.penguinrandomhouse.com/search/site/?q=9780262542623</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Algorithms</t>
+          <t>Annotation</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Panos Louridas</t>
+          <t>https://mitpress.mit.edu/9780262539920/annotation</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/algorithms</t>
+          <t>Remi H. Kalir &amp; Antero Garcia</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>2020-08-18</t>
+          <t>https://mitpress.mit.edu/author/remi-h-kalir-32405 &amp; https://mitpress.mit.edu/author/antero-garcia-22365</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>$15.95</t>
+          <t>April 6, 2021</t>
+        </is>
+      </c>
+      <c r="F31" t="n">
+        <v>232</v>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>$15.95</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>https://www.penguinrandomhouse.com/search/site/?q=9780262539920</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Visual Culture</t>
+          <t>Hate Speech</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Alexis L. Boylan</t>
+          <t>https://mitpress.mit.edu/9780262539906/hate-speech</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/visual-culture-1</t>
+          <t>Caitlin Ring Carlson</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>2020-08-11</t>
+          <t>https://mitpress.mit.edu/author/caitlin-ring-carlson-32570</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>$15.95</t>
+          <t>April 6, 2021</t>
+        </is>
+      </c>
+      <c r="F32" t="n">
+        <v>200</v>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>$15.95</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>https://www.penguinrandomhouse.com/search/site/?q=9780262539906</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Phenomenology</t>
+          <t>Science Fiction</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Chad Engelland</t>
+          <t>https://mitpress.mit.edu/9780262539999/science-fiction</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/phenomenology</t>
+          <t>Sherryl Vint</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>2020-08-04</t>
+          <t>https://mitpress.mit.edu/author/sherryl-vint-29534</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>$15.95</t>
+          <t>February 16, 2021</t>
+        </is>
+      </c>
+      <c r="F33" t="n">
+        <v>224</v>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>$15.95</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>https://www.penguinrandomhouse.com/search/site/?q=9780262539999</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>Anticorruption</t>
+          <t>Ketamine</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Robert I. Rotberg</t>
+          <t>https://mitpress.mit.edu/9780262542241/ketamine</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/anticorruption</t>
+          <t>Bita Moghaddam</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>2020-07-21</t>
+          <t>https://mitpress.mit.edu/author/bita-moghaddam-15562</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>$15.95</t>
+          <t>February 16, 2021</t>
+        </is>
+      </c>
+      <c r="F34" t="n">
+        <v>200</v>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>$15.95</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>https://www.penguinrandomhouse.com/search/site/?q=9780262542241</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Cynicism</t>
+          <t>Recommendation Engines</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>Ansgar Allen</t>
+          <t>https://mitpress.mit.edu/9780262539074/recommendation-engines</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/cynicism</t>
+          <t>Michael Schrage</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>2020-04-14</t>
+          <t>https://mitpress.mit.edu/author/michael-schrage-15361</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>$15.95</t>
+          <t>September 1, 2020</t>
+        </is>
+      </c>
+      <c r="F35" t="n">
+        <v>304</v>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>$15.95</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>https://www.penguinrandomhouse.com/search/site/?q=9780262539074</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Critical Thinking</t>
+          <t>Behavioral Insights</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Jonathan Haber</t>
+          <t>https://mitpress.mit.edu/9780262539401/behavioral-insights</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/critical-thinking</t>
+          <t>Michael Hallsworth &amp; Elspeth Kirkman</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>2020-04-07</t>
+          <t>https://mitpress.mit.edu/author/michael-hallsworth-33251 &amp; https://mitpress.mit.edu/author/elspeth-kirkman-33252</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>$15.95</t>
+          <t>September 1, 2020</t>
+        </is>
+      </c>
+      <c r="F36" t="n">
+        <v>248</v>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>$15.95</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>https://www.penguinrandomhouse.com/search/site/?q=9780262539401</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Extraterrestrials</t>
+          <t>Algorithms</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Wade Roush</t>
+          <t>https://mitpress.mit.edu/9780262539029/algorithms</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/extraterrestrials</t>
+          <t>Panos Louridas</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>2020-04-07</t>
+          <t>https://mitpress.mit.edu/author/panos-louridas-23692</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>$15.95</t>
+          <t>August 18, 2020</t>
+        </is>
+      </c>
+      <c r="F37" t="n">
+        <v>312</v>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>$15.95</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>https://www.penguinrandomhouse.com/search/site/?q=9780262539029</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Contraception</t>
+          <t>Visual Culture</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Donna J. Drucker</t>
+          <t>https://mitpress.mit.edu/9780262539364/visual-culture</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/contraception</t>
+          <t>Alexis L. Boylan</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>2020-04-07</t>
+          <t>https://mitpress.mit.edu/author/alexis-l-boylan-31700</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>$15.95</t>
+          <t>August 11, 2020</t>
+        </is>
+      </c>
+      <c r="F38" t="n">
+        <v>248</v>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>$15.95</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>https://www.penguinrandomhouse.com/search/site/?q=9780262539364</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>AI Ethics</t>
+          <t>Phenomenology</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Mark Coeckelbergh</t>
+          <t>https://mitpress.mit.edu/9780262539319/phenomenology</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/ai-ethics</t>
+          <t>Chad Engelland</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>2020-04-07</t>
+          <t>https://mitpress.mit.edu/author/chad-engelland-21633</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>$15.95</t>
+          <t>August 4, 2020</t>
+        </is>
+      </c>
+      <c r="F39" t="n">
+        <v>264</v>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>$15.95</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>https://www.penguinrandomhouse.com/search/site/?q=9780262539319</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Macroeconomics</t>
+          <t>Anticorruption</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>Felipe Larraín B.</t>
+          <t>https://mitpress.mit.edu/9780262538831/anticorruption</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/macroeconomics</t>
+          <t>Robert I. Rotberg</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>2020-03-17</t>
+          <t>https://mitpress.mit.edu/author/robert-i-rotberg-7442</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>$15.95</t>
+          <t>July 21, 2020</t>
+        </is>
+      </c>
+      <c r="F40" t="n">
+        <v>272</v>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>$15.95</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>https://www.penguinrandomhouse.com/search/site/?q=9780262538831</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>fMRI</t>
+          <t>Cynicism</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Peter A. Bandettini</t>
+          <t>https://mitpress.mit.edu/9780262537889/cynicism</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/fmri</t>
+          <t>Ansgar Allen</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>2020-02-25</t>
+          <t>https://mitpress.mit.edu/author/ansgar-allen-28512</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>$15.95</t>
+          <t>April 14, 2020</t>
+        </is>
+      </c>
+      <c r="F41" t="n">
+        <v>280</v>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>$15.95</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>https://www.penguinrandomhouse.com/search/site/?q=9780262537889</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Collaborative Society</t>
+          <t>Contraception</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>Dariusz Jemielniak, Aleksandra Przegalinska</t>
+          <t>https://mitpress.mit.edu/9780262538428/contraception</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/collaborative-society</t>
+          <t>Donna J. Drucker</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>2020-02-18</t>
+          <t>https://mitpress.mit.edu/author/donna-j-drucker-17704</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>$15.95</t>
+          <t>April 7, 2020</t>
+        </is>
+      </c>
+      <c r="F42" t="n">
+        <v>264</v>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>$15.95</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>https://www.penguinrandomhouse.com/search/site/?q=9780262538428</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Irony and Sarcasm</t>
+          <t>Extraterrestrials</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Roger Kreuz</t>
+          <t>https://mitpress.mit.edu/9780262538435/extraterrestrials</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/irony-and-sarcasm</t>
+          <t>Wade Roush</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>2020-02-18</t>
+          <t>https://mitpress.mit.edu/author/wade-roush-27966</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>$15.95</t>
+          <t>April 7, 2020</t>
+        </is>
+      </c>
+      <c r="F43" t="n">
+        <v>240</v>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>$15.95</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>https://www.penguinrandomhouse.com/search/site/?q=9780262538435</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Quantum Entanglement</t>
+          <t>AI Ethics</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Jed Brody</t>
+          <t>https://mitpress.mit.edu/9780262538190/ai-ethics</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/quantum-entanglement</t>
+          <t>Mark Coeckelbergh</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>2020-02-18</t>
+          <t>https://mitpress.mit.edu/author/mark-coeckelbergh-25812</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>$15.95</t>
+          <t>April 7, 2020</t>
+        </is>
+      </c>
+      <c r="F44" t="n">
+        <v>248</v>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>$15.95</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>https://www.penguinrandomhouse.com/search/site/?q=9780262538190</t>
         </is>
       </c>
     </row>
@@ -1629,22 +2203,35 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Shashi Shekhar, Pamela Vold</t>
+          <t>https://mitpress.mit.edu/9780262538046/spatial-computing</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/spatial-computing</t>
+          <t>Shashi Shekhar &amp; Pamela Vold</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>2020-02-18</t>
+          <t>https://mitpress.mit.edu/author/shashi-shekhar-27374 &amp; https://mitpress.mit.edu/author/pamela-vold-27375</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>$15.95</t>
+          <t>February 18, 2020</t>
+        </is>
+      </c>
+      <c r="F45" t="n">
+        <v>256</v>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>$15.95</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>https://www.penguinrandomhouse.com/search/site/?q=9780262538046</t>
         </is>
       </c>
     </row>
@@ -1656,157 +2243,235 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
+          <t>https://mitpress.mit.edu/9780262538053/smart-cities</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
           <t>Germaine Halegoua</t>
         </is>
       </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>https://mitpress.mit.edu/books/smart-cities</t>
-        </is>
-      </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>2020-02-18</t>
+          <t>https://mitpress.mit.edu/author/germaine-halegoua-17179</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>$15.95</t>
+          <t>February 18, 2020</t>
+        </is>
+      </c>
+      <c r="F46" t="n">
+        <v>248</v>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>$15.95</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>https://www.penguinrandomhouse.com/search/site/?q=9780262538053</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Recycling</t>
+          <t>Quantum Entanglement</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>Finn Arne Jørgensen</t>
+          <t>https://mitpress.mit.edu/9780262538442/quantum-entanglement</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/recycling</t>
+          <t>Jed Brody</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>2019-11-12</t>
+          <t>https://mitpress.mit.edu/author/jed-brody-32281</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>$15.95</t>
+          <t>February 18, 2020</t>
+        </is>
+      </c>
+      <c r="F47" t="n">
+        <v>184</v>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>$15.95</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>https://www.penguinrandomhouse.com/search/site/?q=9780262538442</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Citizenship</t>
+          <t>Irony and Sarcasm</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Dimitry Kochenov</t>
+          <t>https://mitpress.mit.edu/9780262538268/irony-and-sarcasm</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/citizenship</t>
+          <t>Roger Kreuz</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>2019-11-12</t>
+          <t>https://mitpress.mit.edu/author/roger-kreuz-22694</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>$15.95</t>
+          <t>February 18, 2020</t>
+        </is>
+      </c>
+      <c r="F48" t="n">
+        <v>232</v>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>$15.95</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>https://www.penguinrandomhouse.com/search/site/?q=9780262538268</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Fake Photos</t>
+          <t>Recycling</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Hany Farid</t>
+          <t>https://mitpress.mit.edu/9780262537827/recycling</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/fake-photos</t>
+          <t>Finn Arne Jørgensen</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>2019-09-10</t>
+          <t>https://mitpress.mit.edu/author/finn-arne-jorgensen-20224</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>$15.95</t>
+          <t>November 12, 2019</t>
+        </is>
+      </c>
+      <c r="F49" t="n">
+        <v>208</v>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>$15.95</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>https://www.penguinrandomhouse.com/search/site/?q=9780262537827</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Nihilism</t>
+          <t>Citizenship</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Nolen Gertz</t>
+          <t>https://mitpress.mit.edu/9780262537797/citizenship</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/nihilism</t>
+          <t>Dimitry Kochenov</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>2019-09-10</t>
+          <t>https://mitpress.mit.edu/author/dimitry-kochenov-27575</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>$15.95</t>
+          <t>November 12, 2019</t>
+        </is>
+      </c>
+      <c r="F50" t="n">
+        <v>344</v>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>$15.95</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>https://www.penguinrandomhouse.com/search/site/?q=9780262537797</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Virtual Reality</t>
+          <t>Fake Photos</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>Samuel Greengard</t>
+          <t>https://mitpress.mit.edu/9780262537490/fake-photos</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/virtual-reality</t>
+          <t>Hany Farid</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>2019-09-10</t>
+          <t>https://mitpress.mit.edu/author/hany-farid-23716</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>$15.95</t>
+          <t>September 10, 2019</t>
+        </is>
+      </c>
+      <c r="F51" t="n">
+        <v>232</v>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>$15.95</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>https://www.penguinrandomhouse.com/search/site/?q=9780262537490</t>
         </is>
       </c>
     </row>
@@ -1818,211 +2483,315 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
+          <t>https://mitpress.mit.edu/9780262537551/deep-learning</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
           <t>John D. Kelleher</t>
         </is>
       </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>https://mitpress.mit.edu/books/deep-learning-1</t>
-        </is>
-      </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>2019-09-10</t>
+          <t>https://mitpress.mit.edu/author/john-d-kelleher-19876</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>$15.95</t>
+          <t>September 10, 2019</t>
+        </is>
+      </c>
+      <c r="F52" t="n">
+        <v>296</v>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>$15.95</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>https://www.penguinrandomhouse.com/search/site/?q=9780262537551</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Food</t>
+          <t>Nihilism</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Fabio Parasecoli</t>
+          <t>https://mitpress.mit.edu/9780262537179/nihilism</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/food-1</t>
+          <t>Nolen Gertz</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>2019-05-21</t>
+          <t>https://mitpress.mit.edu/author/nolen-gertz-29045</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>$15.95</t>
+          <t>September 10, 2019</t>
+        </is>
+      </c>
+      <c r="F53" t="n">
+        <v>224</v>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>$15.95</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>https://www.penguinrandomhouse.com/search/site/?q=9780262537179</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Computational Thinking</t>
+          <t>Virtual Reality</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Peter J. Denning, Matti Tedre</t>
+          <t>https://mitpress.mit.edu/9780262537520/virtual-reality</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/computational-thinking</t>
+          <t>Samuel Greengard</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>2019-05-14</t>
+          <t>https://mitpress.mit.edu/author/samuel-greengard-22712</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>$15.95</t>
+          <t>September 10, 2019</t>
+        </is>
+      </c>
+      <c r="F54" t="n">
+        <v>264</v>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>$15.95</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>https://www.penguinrandomhouse.com/search/site/?q=9780262537520</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Sexual Consent</t>
+          <t>Food</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Milena Popova</t>
+          <t>https://mitpress.mit.edu/9780262537315/food</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/sexual-consent</t>
+          <t>Fabio Parasecoli</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>2019-05-07</t>
+          <t>https://mitpress.mit.edu/author/fabio-parasecoli-28507</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
         <is>
-          <t>$15.95</t>
+          <t>May 21, 2019</t>
+        </is>
+      </c>
+      <c r="F55" t="n">
+        <v>232</v>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>$15.95</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>https://www.penguinrandomhouse.com/search/site/?q=9780262537315</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>3D Printing</t>
+          <t>Computational Thinking</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>John M. Jordan</t>
+          <t>https://mitpress.mit.edu/9780262536561/computational-thinking</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/3d-printing</t>
+          <t>Peter J. Denning &amp; Matti Tedre</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>2019-03-12</t>
+          <t>https://mitpress.mit.edu/author/peter-j-denning-13845 &amp; https://mitpress.mit.edu/author/matti-tedre-8919</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>$15.95</t>
+          <t>May 14, 2019</t>
+        </is>
+      </c>
+      <c r="F56" t="n">
+        <v>264</v>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>$15.95</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>https://www.penguinrandomhouse.com/search/site/?q=9780262536561</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>GPS</t>
+          <t>Sexual Consent</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Paul E. Ceruzzi</t>
+          <t>https://mitpress.mit.edu/9780262537322/sexual-consent</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/gps</t>
+          <t>Milena Popova</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>2018-11-06</t>
+          <t>https://mitpress.mit.edu/author/milena-popova-31248</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
         <is>
-          <t>$15.95</t>
+          <t>May 7, 2019</t>
+        </is>
+      </c>
+      <c r="F57" t="n">
+        <v>216</v>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>$15.95</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>https://www.penguinrandomhouse.com/search/site/?q=9780262537322</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Spaceflight</t>
+          <t>3D Printing</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Michael J. Neufeld</t>
+          <t>https://mitpress.mit.edu/9780262536684/3d-printing</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/spaceflight</t>
+          <t>John M. Jordan</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>2018-10-16</t>
+          <t>https://mitpress.mit.edu/author/john-m-jordan-24118</t>
         </is>
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>$15.95</t>
+          <t>March 12, 2019</t>
+        </is>
+      </c>
+      <c r="F58" t="n">
+        <v>240</v>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>$15.95</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>https://www.penguinrandomhouse.com/search/site/?q=9780262536684</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>School Choice</t>
+          <t>Spaceflight</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>David R. Garcia</t>
+          <t>https://mitpress.mit.edu/9780262536332/spaceflight</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/school-choice</t>
+          <t>Michael J. Neufeld</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>2018-09-18</t>
+          <t>https://mitpress.mit.edu/author/michael-j-neufeld-27284</t>
         </is>
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>$15.95</t>
+          <t>October 16, 2018</t>
+        </is>
+      </c>
+      <c r="F59" t="n">
+        <v>248</v>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>$15.95</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>https://www.penguinrandomhouse.com/search/site/?q=9780262536332</t>
         </is>
       </c>
     </row>
@@ -2034,886 +2803,435 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
+          <t>https://mitpress.mit.edu/9780262535755/carbon-capture</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
           <t>Howard J. Herzog</t>
         </is>
       </c>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t>https://mitpress.mit.edu/books/carbon-capture</t>
-        </is>
-      </c>
       <c r="D60" t="inlineStr">
         <is>
-          <t>2018-09-11</t>
+          <t>https://mitpress.mit.edu/author/howard-j-herzog-27843</t>
         </is>
       </c>
       <c r="E60" t="inlineStr">
         <is>
+          <t>September 11, 2018</t>
+        </is>
+      </c>
+      <c r="F60" t="n">
+        <v>216</v>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
           <t>$16.95</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>https://www.penguinrandomhouse.com/search/site/?q=9780262535755</t>
         </is>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>Haptics</t>
+          <t>Extremism</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>Lynette Jones</t>
+          <t>https://mitpress.mit.edu/9780262535878/extremism</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/haptics</t>
+          <t>J. M. Berger</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>2018-09-04</t>
+          <t>https://mitpress.mit.edu/author/j-m-berger-28577</t>
         </is>
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>$15.95</t>
+          <t>August 28, 2018</t>
+        </is>
+      </c>
+      <c r="F61" t="n">
+        <v>216</v>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>$16.95</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>https://www.penguinrandomhouse.com/search/site/?q=9780262535878</t>
         </is>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Extremism</t>
+          <t>The Book</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>J. M. Berger</t>
+          <t>https://mitpress.mit.edu/9780262535410/the-book</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/extremism</t>
+          <t>Amaranth Borsuk</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>2018-08-28</t>
+          <t>https://mitpress.mit.edu/author/amaranth-borsuk-24538</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
+          <t>May 4, 2018</t>
+        </is>
+      </c>
+      <c r="F62" t="n">
+        <v>344</v>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
           <t>$16.95</t>
+        </is>
+      </c>
+      <c r="H62" t="inlineStr">
+        <is>
+          <t>https://www.penguinrandomhouse.com/search/site/?q=9780262535410</t>
         </is>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>The Book</t>
+          <t>Data Science</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>Amaranth Borsuk</t>
+          <t>https://mitpress.mit.edu/9780262535434/data-science</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/book</t>
+          <t>John D. Kelleher &amp; Brendan Tierney</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>2018-05-04</t>
+          <t>https://mitpress.mit.edu/author/john-d-kelleher-19876 &amp; https://mitpress.mit.edu/author/brendan-tierney-26222</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
         <is>
-          <t>$16.95</t>
+          <t>April 13, 2018</t>
+        </is>
+      </c>
+      <c r="F63" t="n">
+        <v>280</v>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>$15.95</t>
+        </is>
+      </c>
+      <c r="H63" t="inlineStr">
+        <is>
+          <t>https://www.penguinrandomhouse.com/search/site/?q=9780262535434</t>
         </is>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Data Science</t>
+          <t>Synesthesia</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>John D. Kelleher, Brendan Tierney</t>
+          <t>https://mitpress.mit.edu/9780262535090/synesthesia</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/data-science</t>
+          <t>Richard E. Cytowic</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>2018-04-13</t>
+          <t>https://mitpress.mit.edu/author/richard-e-cytowic-4555</t>
         </is>
       </c>
       <c r="E64" t="inlineStr">
         <is>
-          <t>$15.95</t>
+          <t>March 9, 2018</t>
+        </is>
+      </c>
+      <c r="F64" t="n">
+        <v>288</v>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>$15.95</t>
+        </is>
+      </c>
+      <c r="H64" t="inlineStr">
+        <is>
+          <t>https://www.penguinrandomhouse.com/search/site/?q=9780262535090</t>
         </is>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Synesthesia</t>
+          <t>Post-Truth</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Richard E. Cytowic</t>
+          <t>https://mitpress.mit.edu/9780262535045/post-truth</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/synesthesia</t>
+          <t>Lee McIntyre</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>2018-03-09</t>
+          <t>https://mitpress.mit.edu/author/lee-mcintyre-2985</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>$15.95</t>
+          <t>February 16, 2018</t>
+        </is>
+      </c>
+      <c r="F65" t="n">
+        <v>240</v>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>$15.95</t>
+        </is>
+      </c>
+      <c r="H65" t="inlineStr">
+        <is>
+          <t>https://www.penguinrandomhouse.com/search/site/?q=9780262535045</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Post-Truth</t>
+          <t>Information and Society</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>Lee McIntyre</t>
+          <t>https://mitpress.mit.edu/9780262533386/information-and-society</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/post-truth</t>
+          <t>Michael Buckland</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>2018-02-16</t>
+          <t>https://mitpress.mit.edu/author/michael-buckland-10168</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>$15.95</t>
+          <t>March 3, 2017</t>
+        </is>
+      </c>
+      <c r="F66" t="n">
+        <v>232</v>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>$15.95</t>
+        </is>
+      </c>
+      <c r="H66" t="inlineStr">
+        <is>
+          <t>https://www.penguinrandomhouse.com/search/site/?q=9780262533386</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>The Future</t>
+          <t>MOOCs</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Nick Montfort</t>
+          <t>https://mitpress.mit.edu/9780262526913/moocs</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/future</t>
+          <t>Jonathan Haber</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>2017-12-08</t>
+          <t>https://mitpress.mit.edu/author/jonathan-haber-21957</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>$15.95</t>
+          <t>September 26, 2014</t>
+        </is>
+      </c>
+      <c r="F67" t="n">
+        <v>248</v>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>$15.95</t>
+        </is>
+      </c>
+      <c r="H67" t="inlineStr">
+        <is>
+          <t>https://www.penguinrandomhouse.com/search/site/?q=9780262526913</t>
         </is>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Machine Translation</t>
+          <t>The Conscious Mind</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Thierry Poibeau</t>
+          <t>https://mitpress.mit.edu/9780262527101/the-conscious-mind</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/machine-translation-1</t>
+          <t>Zoltan Torey</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>2017-09-15</t>
+          <t>https://mitpress.mit.edu/author/zoltan-torey-11949</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>$15.95</t>
+          <t>August 8, 2014</t>
+        </is>
+      </c>
+      <c r="F68" t="n">
+        <v>208</v>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>$16.95</t>
+        </is>
+      </c>
+      <c r="H68" t="inlineStr">
+        <is>
+          <t>https://www.penguinrandomhouse.com/search/site/?q=9780262527101</t>
         </is>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Information and Society</t>
+          <t>Free Will</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>Michael Buckland</t>
+          <t>https://mitpress.mit.edu/9780262525794/free-will</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/information-and-society</t>
+          <t>Mark Balaguer</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>2017-03-03</t>
+          <t>https://mitpress.mit.edu/author/mark-balaguer-13441</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>$15.95</t>
+          <t>February 14, 2014</t>
+        </is>
+      </c>
+      <c r="F69" t="n">
+        <v>152</v>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>$15.95</t>
+        </is>
+      </c>
+      <c r="H69" t="inlineStr">
+        <is>
+          <t>https://www.penguinrandomhouse.com/search/site/?q=9780262525794</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Robots</t>
+          <t>Information and the Modern Corporation</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>John M. Jordan</t>
+          <t>https://mitpress.mit.edu/9780262516419/information-and-the-modern-corporation</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>https://mitpress.mit.edu/books/robots</t>
+          <t>James W. Cortada</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>2016-10-14</t>
+          <t>https://mitpress.mit.edu/author/james-w-cortada-5834</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>$15.95</t>
-        </is>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="inlineStr">
-        <is>
-          <t>Machine Learning</t>
-        </is>
-      </c>
-      <c r="B71" t="inlineStr">
-        <is>
-          <t>Ethem Alpaydin</t>
-        </is>
-      </c>
-      <c r="C71" t="inlineStr">
-        <is>
-          <t>https://mitpress.mit.edu/books/machine-learning</t>
-        </is>
-      </c>
-      <c r="D71" t="inlineStr">
-        <is>
-          <t>2016-10-07</t>
-        </is>
-      </c>
-      <c r="E71" t="inlineStr">
-        <is>
-          <t>$15.95</t>
-        </is>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="inlineStr">
-        <is>
-          <t>The Mind–Body Problem</t>
-        </is>
-      </c>
-      <c r="B72" t="inlineStr">
-        <is>
-          <t>Jonathan Westphal</t>
-        </is>
-      </c>
-      <c r="C72" t="inlineStr">
-        <is>
-          <t>https://mitpress.mit.edu/books/mind-body-problem</t>
-        </is>
-      </c>
-      <c r="D72" t="inlineStr">
-        <is>
-          <t>2016-09-30</t>
-        </is>
-      </c>
-      <c r="E72" t="inlineStr">
-        <is>
-          <t>$16.95</t>
-        </is>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="inlineStr">
-        <is>
-          <t>Neuroplasticity</t>
-        </is>
-      </c>
-      <c r="B73" t="inlineStr">
-        <is>
-          <t>Moheb Costandi</t>
-        </is>
-      </c>
-      <c r="C73" t="inlineStr">
-        <is>
-          <t>https://mitpress.mit.edu/books/neuroplasticity</t>
-        </is>
-      </c>
-      <c r="D73" t="inlineStr">
-        <is>
-          <t>2016-08-19</t>
-        </is>
-      </c>
-      <c r="E73" t="inlineStr">
-        <is>
-          <t>$16.95</t>
-        </is>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="inlineStr">
-        <is>
-          <t>Self-Tracking</t>
-        </is>
-      </c>
-      <c r="B74" t="inlineStr">
-        <is>
-          <t>Gina Neff, Dawn Nafus</t>
-        </is>
-      </c>
-      <c r="C74" t="inlineStr">
-        <is>
-          <t>https://mitpress.mit.edu/books/self-tracking</t>
-        </is>
-      </c>
-      <c r="D74" t="inlineStr">
-        <is>
-          <t>2016-06-24</t>
-        </is>
-      </c>
-      <c r="E74" t="inlineStr">
-        <is>
-          <t>$15.95</t>
-        </is>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="inlineStr">
-        <is>
-          <t>Cloud Computing</t>
-        </is>
-      </c>
-      <c r="B75" t="inlineStr">
-        <is>
-          <t>Nayan B. Ruparelia</t>
-        </is>
-      </c>
-      <c r="C75" t="inlineStr">
-        <is>
-          <t>https://mitpress.mit.edu/books/cloud-computing</t>
-        </is>
-      </c>
-      <c r="D75" t="inlineStr">
-        <is>
-          <t>2016-05-13</t>
-        </is>
-      </c>
-      <c r="E75" t="inlineStr">
-        <is>
-          <t>$15.95</t>
-        </is>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="inlineStr">
-        <is>
-          <t>Auctions</t>
-        </is>
-      </c>
-      <c r="B76" t="inlineStr">
-        <is>
-          <t>Timothy P. Hubbard, Harry J. Paarsch</t>
-        </is>
-      </c>
-      <c r="C76" t="inlineStr">
-        <is>
-          <t>https://mitpress.mit.edu/books/auctions</t>
-        </is>
-      </c>
-      <c r="D76" t="inlineStr">
-        <is>
-          <t>2016-01-06</t>
-        </is>
-      </c>
-      <c r="E76" t="inlineStr">
-        <is>
-          <t>$15.95</t>
-        </is>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="inlineStr">
-        <is>
-          <t>Metadata</t>
-        </is>
-      </c>
-      <c r="B77" t="inlineStr">
-        <is>
-          <t>Jeffrey Pomerantz</t>
-        </is>
-      </c>
-      <c r="C77" t="inlineStr">
-        <is>
-          <t>https://mitpress.mit.edu/books/metadata</t>
-        </is>
-      </c>
-      <c r="D77" t="inlineStr">
-        <is>
-          <t>2015-11-06</t>
-        </is>
-      </c>
-      <c r="E77" t="inlineStr">
-        <is>
-          <t>$16.95</t>
-        </is>
-      </c>
-    </row>
-    <row r="78">
-      <c r="A78" t="inlineStr">
-        <is>
-          <t>Sustainability</t>
-        </is>
-      </c>
-      <c r="B78" t="inlineStr">
-        <is>
-          <t>Kent E. Portney</t>
-        </is>
-      </c>
-      <c r="C78" t="inlineStr">
-        <is>
-          <t>https://mitpress.mit.edu/books/sustainability</t>
-        </is>
-      </c>
-      <c r="D78" t="inlineStr">
-        <is>
-          <t>2015-10-09</t>
-        </is>
-      </c>
-      <c r="E78" t="inlineStr">
-        <is>
-          <t>$15.95</t>
-        </is>
-      </c>
-    </row>
-    <row r="79">
-      <c r="A79" t="inlineStr">
-        <is>
-          <t>The Technological Singularity</t>
-        </is>
-      </c>
-      <c r="B79" t="inlineStr">
-        <is>
-          <t>Murray Shanahan</t>
-        </is>
-      </c>
-      <c r="C79" t="inlineStr">
-        <is>
-          <t>https://mitpress.mit.edu/books/technological-singularity</t>
-        </is>
-      </c>
-      <c r="D79" t="inlineStr">
-        <is>
-          <t>2015-08-07</t>
-        </is>
-      </c>
-      <c r="E79" t="inlineStr">
-        <is>
-          <t>$16.95</t>
-        </is>
-      </c>
-    </row>
-    <row r="80">
-      <c r="A80" t="inlineStr">
-        <is>
-          <t>The Internet of Things</t>
-        </is>
-      </c>
-      <c r="B80" t="inlineStr">
-        <is>
-          <t>Samuel Greengard</t>
-        </is>
-      </c>
-      <c r="C80" t="inlineStr">
-        <is>
-          <t>https://mitpress.mit.edu/books/internet-things</t>
-        </is>
-      </c>
-      <c r="D80" t="inlineStr">
-        <is>
-          <t>2015-03-20</t>
-        </is>
-      </c>
-      <c r="E80" t="inlineStr">
-        <is>
-          <t>$15.95</t>
-        </is>
-      </c>
-    </row>
-    <row r="81">
-      <c r="A81" t="inlineStr">
-        <is>
-          <t>MOOCs</t>
-        </is>
-      </c>
-      <c r="B81" t="inlineStr">
-        <is>
-          <t>Jonathan Haber</t>
-        </is>
-      </c>
-      <c r="C81" t="inlineStr">
-        <is>
-          <t>https://mitpress.mit.edu/books/moocs</t>
-        </is>
-      </c>
-      <c r="D81" t="inlineStr">
-        <is>
-          <t>2014-09-26</t>
-        </is>
-      </c>
-      <c r="E81" t="inlineStr">
-        <is>
-          <t>$15.95</t>
-        </is>
-      </c>
-    </row>
-    <row r="82">
-      <c r="A82" t="inlineStr">
-        <is>
-          <t>Understanding Beliefs</t>
-        </is>
-      </c>
-      <c r="B82" t="inlineStr">
-        <is>
-          <t>Nils J. Nilsson</t>
-        </is>
-      </c>
-      <c r="C82" t="inlineStr">
-        <is>
-          <t>https://mitpress.mit.edu/books/understanding-beliefs</t>
-        </is>
-      </c>
-      <c r="D82" t="inlineStr">
-        <is>
-          <t>2014-08-15</t>
-        </is>
-      </c>
-      <c r="E82" t="inlineStr">
-        <is>
-          <t>$16.95</t>
-        </is>
-      </c>
-    </row>
-    <row r="83">
-      <c r="A83" t="inlineStr">
-        <is>
-          <t>The Conscious Mind</t>
-        </is>
-      </c>
-      <c r="B83" t="inlineStr">
-        <is>
-          <t>Zoltan Torey</t>
-        </is>
-      </c>
-      <c r="C83" t="inlineStr">
-        <is>
-          <t>https://mitpress.mit.edu/books/conscious-mind</t>
-        </is>
-      </c>
-      <c r="D83" t="inlineStr">
-        <is>
-          <t>2014-08-08</t>
-        </is>
-      </c>
-      <c r="E83" t="inlineStr">
-        <is>
-          <t>$16.95</t>
-        </is>
-      </c>
-    </row>
-    <row r="84">
-      <c r="A84" t="inlineStr">
-        <is>
-          <t>Paradox</t>
-        </is>
-      </c>
-      <c r="B84" t="inlineStr">
-        <is>
-          <t>Margaret Cuonzo</t>
-        </is>
-      </c>
-      <c r="C84" t="inlineStr">
-        <is>
-          <t>https://mitpress.mit.edu/books/paradox</t>
-        </is>
-      </c>
-      <c r="D84" t="inlineStr">
-        <is>
-          <t>2014-02-14</t>
-        </is>
-      </c>
-      <c r="E84" t="inlineStr">
-        <is>
-          <t>$15.95</t>
-        </is>
-      </c>
-    </row>
-    <row r="85">
-      <c r="A85" t="inlineStr">
-        <is>
-          <t>Free Will</t>
-        </is>
-      </c>
-      <c r="B85" t="inlineStr">
-        <is>
-          <t>Mark Balaguer</t>
-        </is>
-      </c>
-      <c r="C85" t="inlineStr">
-        <is>
-          <t>https://mitpress.mit.edu/books/free-will</t>
-        </is>
-      </c>
-      <c r="D85" t="inlineStr">
-        <is>
-          <t>2014-02-14</t>
-        </is>
-      </c>
-      <c r="E85" t="inlineStr">
-        <is>
-          <t>$15.95</t>
-        </is>
-      </c>
-    </row>
-    <row r="86">
-      <c r="A86" t="inlineStr">
-        <is>
-          <t>Memes in Digital Culture</t>
-        </is>
-      </c>
-      <c r="B86" t="inlineStr">
-        <is>
-          <t>Limor Shifman</t>
-        </is>
-      </c>
-      <c r="C86" t="inlineStr">
-        <is>
-          <t>https://mitpress.mit.edu/books/memes-digital-culture</t>
-        </is>
-      </c>
-      <c r="D86" t="inlineStr">
-        <is>
-          <t>2013-10-04</t>
-        </is>
-      </c>
-      <c r="E86" t="inlineStr">
-        <is>
-          <t>$15.95</t>
-        </is>
-      </c>
-    </row>
-    <row r="87">
-      <c r="A87" t="inlineStr">
-        <is>
-          <t>Crowdsourcing</t>
-        </is>
-      </c>
-      <c r="B87" t="inlineStr">
-        <is>
-          <t>Daren C. Brabham</t>
-        </is>
-      </c>
-      <c r="C87" t="inlineStr">
-        <is>
-          <t>https://mitpress.mit.edu/books/crowdsourcing</t>
-        </is>
-      </c>
-      <c r="D87" t="inlineStr">
-        <is>
-          <t>2013-05-10</t>
-        </is>
-      </c>
-      <c r="E87" t="inlineStr">
-        <is>
-          <t>$15.95</t>
-        </is>
-      </c>
-    </row>
-    <row r="88">
-      <c r="A88" t="inlineStr">
-        <is>
-          <t>Waves</t>
-        </is>
-      </c>
-      <c r="B88" t="inlineStr">
-        <is>
-          <t>Fredric Raichlen</t>
-        </is>
-      </c>
-      <c r="C88" t="inlineStr">
-        <is>
-          <t>https://mitpress.mit.edu/books/waves</t>
-        </is>
-      </c>
-      <c r="D88" t="inlineStr">
-        <is>
-          <t>2012-10-19</t>
-        </is>
-      </c>
-      <c r="E88" t="inlineStr">
-        <is>
-          <t>$16.95</t>
-        </is>
-      </c>
-    </row>
-    <row r="89">
-      <c r="A89" t="inlineStr">
-        <is>
-          <t>Open Access</t>
-        </is>
-      </c>
-      <c r="B89" t="inlineStr">
-        <is>
-          <t>Peter Suber</t>
-        </is>
-      </c>
-      <c r="C89" t="inlineStr">
-        <is>
-          <t>https://mitpress.mit.edu/books/open-access</t>
-        </is>
-      </c>
-      <c r="D89" t="inlineStr">
-        <is>
-          <t>2012-07-20</t>
-        </is>
-      </c>
-      <c r="E89" t="inlineStr">
-        <is>
-          <t>$15.95</t>
-        </is>
-      </c>
-    </row>
-    <row r="90">
-      <c r="A90" t="inlineStr">
-        <is>
-          <t>Computing</t>
-        </is>
-      </c>
-      <c r="B90" t="inlineStr">
-        <is>
-          <t>Paul E. Ceruzzi</t>
-        </is>
-      </c>
-      <c r="C90" t="inlineStr">
-        <is>
-          <t>https://mitpress.mit.edu/books/computing-1</t>
-        </is>
-      </c>
-      <c r="D90" t="inlineStr">
-        <is>
-          <t>2012-06-15</t>
-        </is>
-      </c>
-      <c r="E90" t="inlineStr">
-        <is>
-          <t>$16.95</t>
-        </is>
-      </c>
-    </row>
-    <row r="91">
-      <c r="A91" t="inlineStr">
-        <is>
-          <t>Information and the Modern Corporation</t>
-        </is>
-      </c>
-      <c r="B91" t="inlineStr">
-        <is>
-          <t>James W. Cortada</t>
-        </is>
-      </c>
-      <c r="C91" t="inlineStr">
-        <is>
-          <t>https://mitpress.mit.edu/books/information-and-modern-corporation</t>
-        </is>
-      </c>
-      <c r="D91" t="inlineStr">
-        <is>
-          <t>2011-10-07</t>
-        </is>
-      </c>
-      <c r="E91" t="inlineStr">
-        <is>
-          <t>$15.95</t>
-        </is>
-      </c>
-    </row>
-    <row r="92">
-      <c r="A92" t="inlineStr">
-        <is>
-          <t>Intellectual Property Strategy</t>
-        </is>
-      </c>
-      <c r="B92" t="inlineStr">
-        <is>
-          <t>John Palfrey</t>
-        </is>
-      </c>
-      <c r="C92" t="inlineStr">
-        <is>
-          <t>https://mitpress.mit.edu/books/intellectual-property-strategy</t>
-        </is>
-      </c>
-      <c r="D92" t="inlineStr">
-        <is>
-          <t>2011-10-07</t>
-        </is>
-      </c>
-      <c r="E92" t="inlineStr">
-        <is>
-          <t>$15.95</t>
+          <t>October 7, 2011</t>
+        </is>
+      </c>
+      <c r="F70" t="n">
+        <v>176</v>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>$15.95</t>
+        </is>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>https://www.penguinrandomhouse.com/search/site/?q=9780262516419</t>
         </is>
       </c>
     </row>

</xml_diff>